<commit_message>
Verizon Wireless - Protect Your Enterprise Page - 10 Test Cases Done
</commit_message>
<xml_diff>
--- a/verizonWireless/src/main/resources/VerizonWireless_ProtectYourEnterprisePage_ExpectedElements.xlsx
+++ b/verizonWireless/src/main/resources/VerizonWireless_ProtectYourEnterprisePage_ExpectedElements.xlsx
@@ -9,11 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" firstSheet="7" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="PageConfirmText" sheetId="1" r:id="rId1"/>
     <sheet name="DropdownProtectEnt Count" sheetId="2" r:id="rId2"/>
+    <sheet name="DropdownProtectEnt Names" sheetId="3" r:id="rId3"/>
+    <sheet name="DropdownProtectEnt URLs" sheetId="4" r:id="rId4"/>
+    <sheet name="NavBar Names" sheetId="5" r:id="rId5"/>
+    <sheet name="GridContainerOne Titles" sheetId="6" r:id="rId6"/>
+    <sheet name="GridContainerOne Sec1 Body" sheetId="7" r:id="rId7"/>
+    <sheet name="GridContainerOne Sec2 Body" sheetId="8" r:id="rId8"/>
+    <sheet name="ContactUs URL" sheetId="9" r:id="rId9"/>
+    <sheet name="ExpandStack Titles" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,9 +33,120 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Protect your enterprise from threats.</t>
+  </si>
+  <si>
+    <t>Global Integrated Solutions</t>
+  </si>
+  <si>
+    <t>Adapt and transform your business</t>
+  </si>
+  <si>
+    <t>Industries</t>
+  </si>
+  <si>
+    <t>Customer Success Stories</t>
+  </si>
+  <si>
+    <t>Public Sector</t>
+  </si>
+  <si>
+    <t>Adapt-Elevate-Innovate</t>
+  </si>
+  <si>
+    <t>Personalize your customer experience</t>
+  </si>
+  <si>
+    <t>Capitalize on your valuable data</t>
+  </si>
+  <si>
+    <t>https://enterprise.verizon.com/solutions/global-integrated-solutions/</t>
+  </si>
+  <si>
+    <t>https://enterprise.verizon.com/solutions/adapt-and-transform-your-business/</t>
+  </si>
+  <si>
+    <t>https://enterprise.verizon.com/solutions/capitalize-on-your-valuable-data/</t>
+  </si>
+  <si>
+    <t>https://enterprise.verizon.com/solutions/personalize-your-customer-experience/</t>
+  </si>
+  <si>
+    <t>https://enterprise.verizon.com/solutions/industry/</t>
+  </si>
+  <si>
+    <t>https://enterprise.verizon.com/solutions/public-sector/</t>
+  </si>
+  <si>
+    <t>https://enterprise.verizon.com/solutions/adapt-elevate-innovate/</t>
+  </si>
+  <si>
+    <t>https://enterprise.verizon.com/solutions/customer-success-stories/?page=1</t>
+  </si>
+  <si>
+    <t>Your environment</t>
+  </si>
+  <si>
+    <t>Verizon's approach</t>
+  </si>
+  <si>
+    <t>Our capabilities</t>
+  </si>
+  <si>
+    <t>Products &amp; services</t>
+  </si>
+  <si>
+    <t>Managed &amp; professional services</t>
+  </si>
+  <si>
+    <t>New &amp; noteworthy</t>
+  </si>
+  <si>
+    <t>Secure your
+attack surface.</t>
+  </si>
+  <si>
+    <t>Let's talk
+cybersecurity.</t>
+  </si>
+  <si>
+    <t>The world grows more connected every day. Each connection is like an open invitation to attackers looking to breach your business. As your attack surface grows, managing risk becomes more important—and complex. You need intelligent insights into your risk posture and a cybersecurity strategy to help you secure every access point, from the core to the edge. We can help you build it.</t>
+  </si>
+  <si>
+    <t>Integrating the right end-to-end security program is a complex proposition. We help make it easier by working with you to identify your vulnerabilities, and to design a cybersecurity strategy that addresses them. Our cybersecurity expertise can support security program integration across your enterprise—from your network's core to devices at the edge.</t>
+  </si>
+  <si>
+    <t>https://enterprise.verizon.com/support/sales/</t>
+  </si>
+  <si>
+    <t>Mitigate
+risk by
+understanding
+it.</t>
+  </si>
+  <si>
+    <t>Protect your
+business
+with program
+monitoring and
+management.</t>
+  </si>
+  <si>
+    <t>Prepare for
+and respond
+to the worst-
+case
+scenario.</t>
+  </si>
+  <si>
+    <t>Address
+enterprise
+security
+from the
+core to the
+edge.</t>
   </si>
 </sst>
 </file>
@@ -63,8 +182,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -364,13 +486,49 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -382,4 +540,249 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
VerizonWireless - Protect Your Enterprise Page - 20 Test Cases DONE
</commit_message>
<xml_diff>
--- a/verizonWireless/src/main/resources/VerizonWireless_ProtectYourEnterprisePage_ExpectedElements.xlsx
+++ b/verizonWireless/src/main/resources/VerizonWireless_ProtectYourEnterprisePage_ExpectedElements.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" firstSheet="7" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" firstSheet="17" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="PageConfirmText" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,18 @@
     <sheet name="GridContainerOne Sec1 Body" sheetId="7" r:id="rId7"/>
     <sheet name="GridContainerOne Sec2 Body" sheetId="8" r:id="rId8"/>
     <sheet name="ContactUs URL" sheetId="9" r:id="rId9"/>
-    <sheet name="ExpandStack Titles" sheetId="10" r:id="rId10"/>
+    <sheet name="ExpandStack Title1" sheetId="10" r:id="rId10"/>
+    <sheet name="ExpandStack Title2" sheetId="13" r:id="rId11"/>
+    <sheet name="ExpandStack Title3" sheetId="14" r:id="rId12"/>
+    <sheet name="ExpandStack Title4" sheetId="15" r:id="rId13"/>
+    <sheet name="ExpandStack TextTitle1" sheetId="11" r:id="rId14"/>
+    <sheet name="ExpandStack TextTitle2" sheetId="16" r:id="rId15"/>
+    <sheet name="ExpandStack TextTitle3" sheetId="17" r:id="rId16"/>
+    <sheet name="ExpandStack TextTitle4" sheetId="18" r:id="rId17"/>
+    <sheet name="ExpandStack TextBody1" sheetId="12" r:id="rId18"/>
+    <sheet name="ExpandStack TextBody2" sheetId="19" r:id="rId19"/>
+    <sheet name="ExpandStack TextBody3" sheetId="20" r:id="rId20"/>
+    <sheet name="ExpandStack TextBody4" sheetId="21" r:id="rId21"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -33,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>Protect your enterprise from threats.</t>
   </si>
@@ -121,32 +132,74 @@
     <t>https://enterprise.verizon.com/support/sales/</t>
   </si>
   <si>
+    <t>Understand the cybersecurity landscape, trends in breach behavior and how they affect your assets.</t>
+  </si>
+  <si>
+    <t>Understand the global breach landscape and how to interpret its data.</t>
+  </si>
+  <si>
+    <t>Use enterprise-specific risk posture data to make intelligence-driven investments.</t>
+  </si>
+  <si>
+    <t>Take advantage of professional services resources to build a blueprint for security.</t>
+  </si>
+  <si>
+    <t>Secure data in transit and across all access points, including cloud, mobile and IoT.</t>
+  </si>
+  <si>
+    <t>Respond to opportunities and implement changes quickly with virtualized network options.</t>
+  </si>
+  <si>
+    <t>Defend against security risks with advanced threat detection and incident response capabilities.</t>
+  </si>
+  <si>
+    <t>Better control overhead and operational expenses through intelligence-driven security monitoring.</t>
+  </si>
+  <si>
+    <t>Address gaps in security program expertise by using managed program resources.</t>
+  </si>
+  <si>
+    <t>Secure data access points with the right access and identity management safeguards.</t>
+  </si>
+  <si>
     <t>Mitigate
-risk by
-understanding
-it.</t>
+ risk by
+ understanding
+ it.</t>
   </si>
   <si>
     <t>Protect your
-business
-with program
-monitoring and
-management.</t>
+ business
+ with program
+ monitoring and
+ management.</t>
   </si>
   <si>
     <t>Prepare for
-and respond
-to the worst-
+ and respond
+ to the worst-
 case
-scenario.</t>
+ scenario.</t>
   </si>
   <si>
     <t>Address
-enterprise
-security
-from the
-core to the
+ enterprise
+ security
+ from the
+ core to the 
 edge.</t>
+  </si>
+  <si>
+    <t>Address risk, vulnerability and business continuity at the network level.</t>
+  </si>
+  <si>
+    <t>We'll help you create a comprehensive approach that mitigates risk across your enterprise.</t>
+  </si>
+  <si>
+    <t>We'll show you the value of incident detection, response and long-term program management.</t>
+  </si>
+  <si>
+    <t>&lt;a data-loc="Content:Link:assets" class="vz-text-link" href="https://enterprise.verizon.com/resources/learn-the-basics/top-cloud-security-risks-today/"&gt;Understand the top cloud security risks affecting enterprises today.&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -488,39 +541,239 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="91.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="218.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -535,6 +788,71 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -703,7 +1021,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,7 +1049,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>